<commit_message>
Leaves Balance Automation commit 1st
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Leave_Settings_TestData.xlsx
+++ b/src/main/resources/TestData/Leave_Settings_TestData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC_01" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TC_02" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -89,10 +90,10 @@
     <t xml:space="preserve">Is this a Special Leave_CheckBox</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify_Admin_is_able_to_edit_policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All Disable</t>
+    <t xml:space="preserve">Verify_Admin_can_create_Leave_Policies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal Leave Policy</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
@@ -104,52 +105,61 @@
     <t xml:space="preserve">Automation_Test_Description</t>
   </si>
   <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday, Tuesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation_Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male Only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit on Pro-Rata basis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro-rata No, Accural No Leave Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave Type for Automatioon Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave_Type_For_Automation_Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
     <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Financial Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monday, Tuesday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation_Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male Only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, Dadar Mumbai, Middle Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animation </t>
   </si>
 </sst>
 </file>
@@ -159,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -195,6 +205,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -238,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +263,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,34 +289,35 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,56 +404,56 @@
       <c r="E2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="M2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="P2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -452,25 +472,281 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>41</v>
-      </c>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushed after merging latest architect
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Leave_Settings_TestData.xlsx
+++ b/src/main/resources/TestData/Leave_Settings_TestData.xlsx
@@ -10,7 +10,8 @@
   <sheets>
     <sheet name="TC_01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TC_02" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="TC_0211" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -169,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -204,11 +205,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -266,7 +262,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,29 +291,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="48.5969387755102"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,24 +468,118 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.76530612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6683673469388"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4387755102041"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,6 +610,246 @@
       <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="ACQ1" s="0"/>
+      <c r="ACR1" s="0"/>
+      <c r="ACS1" s="0"/>
+      <c r="ACT1" s="0"/>
+      <c r="ACU1" s="0"/>
+      <c r="ACV1" s="0"/>
+      <c r="ACW1" s="0"/>
+      <c r="ACX1" s="0"/>
+      <c r="ACY1" s="0"/>
+      <c r="ACZ1" s="0"/>
+      <c r="ADA1" s="0"/>
+      <c r="ADB1" s="0"/>
+      <c r="ADC1" s="0"/>
+      <c r="ADD1" s="0"/>
+      <c r="ADE1" s="0"/>
+      <c r="ADF1" s="0"/>
+      <c r="ADG1" s="0"/>
+      <c r="ADH1" s="0"/>
+      <c r="ADI1" s="0"/>
+      <c r="ADJ1" s="0"/>
+      <c r="ADK1" s="0"/>
+      <c r="ADL1" s="0"/>
+      <c r="ADM1" s="0"/>
+      <c r="ADN1" s="0"/>
+      <c r="ADO1" s="0"/>
+      <c r="ADP1" s="0"/>
+      <c r="ADQ1" s="0"/>
+      <c r="ADR1" s="0"/>
+      <c r="ADS1" s="0"/>
+      <c r="ADT1" s="0"/>
+      <c r="ADU1" s="0"/>
+      <c r="ADV1" s="0"/>
+      <c r="ADW1" s="0"/>
+      <c r="ADX1" s="0"/>
+      <c r="ADY1" s="0"/>
+      <c r="ADZ1" s="0"/>
+      <c r="AEA1" s="0"/>
+      <c r="AEB1" s="0"/>
+      <c r="AEC1" s="0"/>
+      <c r="AED1" s="0"/>
+      <c r="AEE1" s="0"/>
+      <c r="AEF1" s="0"/>
+      <c r="AEG1" s="0"/>
+      <c r="AEH1" s="0"/>
+      <c r="AEI1" s="0"/>
+      <c r="AEJ1" s="0"/>
+      <c r="AEK1" s="0"/>
+      <c r="AEL1" s="0"/>
+      <c r="AEM1" s="0"/>
+      <c r="AEN1" s="0"/>
+      <c r="AEO1" s="0"/>
+      <c r="AEP1" s="0"/>
+      <c r="AEQ1" s="0"/>
+      <c r="AER1" s="0"/>
+      <c r="AES1" s="0"/>
+      <c r="AET1" s="0"/>
+      <c r="AEU1" s="0"/>
+      <c r="AEV1" s="0"/>
+      <c r="AEW1" s="0"/>
+      <c r="AEX1" s="0"/>
+      <c r="AEY1" s="0"/>
+      <c r="AEZ1" s="0"/>
+      <c r="AFA1" s="0"/>
+      <c r="AFB1" s="0"/>
+      <c r="AFC1" s="0"/>
+      <c r="AFD1" s="0"/>
+      <c r="AFE1" s="0"/>
+      <c r="AFF1" s="0"/>
+      <c r="AFG1" s="0"/>
+      <c r="AFH1" s="0"/>
+      <c r="AFI1" s="0"/>
+      <c r="AFJ1" s="0"/>
+      <c r="AFK1" s="0"/>
+      <c r="AFL1" s="0"/>
+      <c r="AFM1" s="0"/>
+      <c r="AFN1" s="0"/>
+      <c r="AFO1" s="0"/>
+      <c r="AFP1" s="0"/>
+      <c r="AFQ1" s="0"/>
+      <c r="AFR1" s="0"/>
+      <c r="AFS1" s="0"/>
+      <c r="AFT1" s="0"/>
+      <c r="AFU1" s="0"/>
+      <c r="AFV1" s="0"/>
+      <c r="AFW1" s="0"/>
+      <c r="AFX1" s="0"/>
+      <c r="AFY1" s="0"/>
+      <c r="AFZ1" s="0"/>
+      <c r="AGA1" s="0"/>
+      <c r="AGB1" s="0"/>
+      <c r="AGC1" s="0"/>
+      <c r="AGD1" s="0"/>
+      <c r="AGE1" s="0"/>
+      <c r="AGF1" s="0"/>
+      <c r="AGG1" s="0"/>
+      <c r="AGH1" s="0"/>
+      <c r="AGI1" s="0"/>
+      <c r="AGJ1" s="0"/>
+      <c r="AGK1" s="0"/>
+      <c r="AGL1" s="0"/>
+      <c r="AGM1" s="0"/>
+      <c r="AGN1" s="0"/>
+      <c r="AGO1" s="0"/>
+      <c r="AGP1" s="0"/>
+      <c r="AGQ1" s="0"/>
+      <c r="AGR1" s="0"/>
+      <c r="AGS1" s="0"/>
+      <c r="AGT1" s="0"/>
+      <c r="AGU1" s="0"/>
+      <c r="AGV1" s="0"/>
+      <c r="AGW1" s="0"/>
+      <c r="AGX1" s="0"/>
+      <c r="AGY1" s="0"/>
+      <c r="AGZ1" s="0"/>
+      <c r="AHA1" s="0"/>
+      <c r="AHB1" s="0"/>
+      <c r="AHC1" s="0"/>
+      <c r="AHD1" s="0"/>
+      <c r="AHE1" s="0"/>
+      <c r="AHF1" s="0"/>
+      <c r="AHG1" s="0"/>
+      <c r="AHH1" s="0"/>
+      <c r="AHI1" s="0"/>
+      <c r="AHJ1" s="0"/>
+      <c r="AHK1" s="0"/>
+      <c r="AHL1" s="0"/>
+      <c r="AHM1" s="0"/>
+      <c r="AHN1" s="0"/>
+      <c r="AHO1" s="0"/>
+      <c r="AHP1" s="0"/>
+      <c r="AHQ1" s="0"/>
+      <c r="AHR1" s="0"/>
+      <c r="AHS1" s="0"/>
+      <c r="AHT1" s="0"/>
+      <c r="AHU1" s="0"/>
+      <c r="AHV1" s="0"/>
+      <c r="AHW1" s="0"/>
+      <c r="AHX1" s="0"/>
+      <c r="AHY1" s="0"/>
+      <c r="AHZ1" s="0"/>
+      <c r="AIA1" s="0"/>
+      <c r="AIB1" s="0"/>
+      <c r="AIC1" s="0"/>
+      <c r="AID1" s="0"/>
+      <c r="AIE1" s="0"/>
+      <c r="AIF1" s="0"/>
+      <c r="AIG1" s="0"/>
+      <c r="AIH1" s="0"/>
+      <c r="AII1" s="0"/>
+      <c r="AIJ1" s="0"/>
+      <c r="AIK1" s="0"/>
+      <c r="AIL1" s="0"/>
+      <c r="AIM1" s="0"/>
+      <c r="AIN1" s="0"/>
+      <c r="AIO1" s="0"/>
+      <c r="AIP1" s="0"/>
+      <c r="AIQ1" s="0"/>
+      <c r="AIR1" s="0"/>
+      <c r="AIS1" s="0"/>
+      <c r="AIT1" s="0"/>
+      <c r="AIU1" s="0"/>
+      <c r="AIV1" s="0"/>
+      <c r="AIW1" s="0"/>
+      <c r="AIX1" s="0"/>
+      <c r="AIY1" s="0"/>
+      <c r="AIZ1" s="0"/>
+      <c r="AJA1" s="0"/>
+      <c r="AJB1" s="0"/>
+      <c r="AJC1" s="0"/>
+      <c r="AJD1" s="0"/>
+      <c r="AJE1" s="0"/>
+      <c r="AJF1" s="0"/>
+      <c r="AJG1" s="0"/>
+      <c r="AJH1" s="0"/>
+      <c r="AJI1" s="0"/>
+      <c r="AJJ1" s="0"/>
+      <c r="AJK1" s="0"/>
+      <c r="AJL1" s="0"/>
+      <c r="AJM1" s="0"/>
+      <c r="AJN1" s="0"/>
+      <c r="AJO1" s="0"/>
+      <c r="AJP1" s="0"/>
+      <c r="AJQ1" s="0"/>
+      <c r="AJR1" s="0"/>
+      <c r="AJS1" s="0"/>
+      <c r="AJT1" s="0"/>
+      <c r="AJU1" s="0"/>
+      <c r="AJV1" s="0"/>
+      <c r="AJW1" s="0"/>
+      <c r="AJX1" s="0"/>
+      <c r="AJY1" s="0"/>
+      <c r="AJZ1" s="0"/>
+      <c r="AKA1" s="0"/>
+      <c r="AKB1" s="0"/>
+      <c r="AKC1" s="0"/>
+      <c r="AKD1" s="0"/>
+      <c r="AKE1" s="0"/>
+      <c r="AKF1" s="0"/>
+      <c r="AKG1" s="0"/>
+      <c r="AKH1" s="0"/>
+      <c r="AKI1" s="0"/>
+      <c r="AKJ1" s="0"/>
+      <c r="AKK1" s="0"/>
+      <c r="AKL1" s="0"/>
+      <c r="AKM1" s="0"/>
+      <c r="AKN1" s="0"/>
+      <c r="AKO1" s="0"/>
+      <c r="AKP1" s="0"/>
+      <c r="AKQ1" s="0"/>
+      <c r="AKR1" s="0"/>
+      <c r="AKS1" s="0"/>
+      <c r="AKT1" s="0"/>
+      <c r="AKU1" s="0"/>
+      <c r="AKV1" s="0"/>
+      <c r="AKW1" s="0"/>
+      <c r="AKX1" s="0"/>
+      <c r="AKY1" s="0"/>
+      <c r="AKZ1" s="0"/>
+      <c r="ALA1" s="0"/>
+      <c r="ALB1" s="0"/>
+      <c r="ALC1" s="0"/>
+      <c r="ALD1" s="0"/>
+      <c r="ALE1" s="0"/>
+      <c r="ALF1" s="0"/>
+      <c r="ALG1" s="0"/>
+      <c r="ALH1" s="0"/>
+      <c r="ALI1" s="0"/>
+      <c r="ALJ1" s="0"/>
+      <c r="ALK1" s="0"/>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
       <c r="ALW1" s="0"/>
       <c r="ALX1" s="0"/>
       <c r="ALY1" s="0"/>
@@ -575,7 +905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -588,29 +918,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="48.5969387755102"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Leave Balance Calculation Automation Done, Request for PR
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Leave_Settings_TestData.xlsx
+++ b/src/main/resources/TestData/Leave_Settings_TestData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC_01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TC_02" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="TC_0211" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="TC_03" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="TC_0211" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -151,13 +152,22 @@
     <t xml:space="preserve">Pro-rata No, Accural No Leave Policy</t>
   </si>
   <si>
+    <t xml:space="preserve">Leave Type for Automation Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave_Type_For_Automation_Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Leave Balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For a Particular Scenario</t>
+  </si>
+  <si>
     <t xml:space="preserve">Leave Type for Automatioon Testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leave_Type_For_Automation_Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">32</t>
@@ -291,29 +301,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="47.9234693877551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="47.2448979591837"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,22 +480,22 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.76530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,24 +572,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.76530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +955,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>24</v>
@@ -905,42 +981,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="47.9234693877551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="47.2448979591837"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,7 +1104,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>27</v>

</xml_diff>